<commit_message>
commented the codes and changes iin excel file
</commit_message>
<xml_diff>
--- a/BankingProjectPrac/PractiseProjectActitime/Resources/demodata.xlsx
+++ b/BankingProjectPrac/PractiseProjectActitime/Resources/demodata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\source\repos\BankingProjectPrac\BankingProjectPrac\PractiseProjectActitime\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13671DCD-FA41-47EC-BA58-C6BAFF1B1CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B34CE40-851D-44CD-A15F-202FA12CAB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{F0820AA5-5A07-4BD5-9330-A644BABDB898}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>url</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>manager</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +434,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>